<commit_message>
Hello my commit .......
Domooooooooooooo!!!!!!!!11
</commit_message>
<xml_diff>
--- a/format-doc.xlsx
+++ b/format-doc.xlsx
@@ -6,14 +6,14 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -43,72 +43,6 @@
   </si>
   <si>
     <t>ana</t>
-  </si>
-  <si>
-    <t>CGS24003</t>
-  </si>
-  <si>
-    <t>raf</t>
-  </si>
-  <si>
-    <t>CGS24004</t>
-  </si>
-  <si>
-    <t>0xff</t>
-  </si>
-  <si>
-    <t>CGS24005</t>
-  </si>
-  <si>
-    <t>CGS24006</t>
-  </si>
-  <si>
-    <t>CGS24007</t>
-  </si>
-  <si>
-    <t>CGS24008</t>
-  </si>
-  <si>
-    <t>CGS24009</t>
-  </si>
-  <si>
-    <t>CGS24010</t>
-  </si>
-  <si>
-    <t>CGS24011</t>
-  </si>
-  <si>
-    <t>CGS24012</t>
-  </si>
-  <si>
-    <t>CGS24013</t>
-  </si>
-  <si>
-    <t>CGS24014</t>
-  </si>
-  <si>
-    <t>CGS24015</t>
-  </si>
-  <si>
-    <t>CGS24016</t>
-  </si>
-  <si>
-    <t>CGS24017</t>
-  </si>
-  <si>
-    <t>CGS24018</t>
-  </si>
-  <si>
-    <t>CGS24019</t>
-  </si>
-  <si>
-    <t>CGS24020</t>
-  </si>
-  <si>
-    <t>CGS24021</t>
-  </si>
-  <si>
-    <t>CGS24022</t>
   </si>
 </sst>
 </file>
@@ -148,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -162,6 +96,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -722,284 +657,124 @@
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" ht="14.25"/>
   </sheetData>

</xml_diff>